<commit_message>
Updated Excel and XcelUtil
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/UsersAPI.xlsx
+++ b/src/test/resources/exceldata/UsersAPI.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star\git\DieticianAPI-Hackathon\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C6F86E-87AD-4CDF-9852-1C8D8F6FA540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B8DBFD-AE0D-4B7B-A6A7-5A0C0FBDE8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
   </bookViews>
   <sheets>
-    <sheet name="PostUsersExistOneField" sheetId="2" r:id="rId1"/>
-    <sheet name="PostUsers" sheetId="1" r:id="rId2"/>
+    <sheet name="PostUsers" sheetId="1" r:id="rId1"/>
+    <sheet name="PostUsersExistOneField" sheetId="2" r:id="rId2"/>
     <sheet name="PostUsersUserType" sheetId="4" r:id="rId3"/>
     <sheet name="PostUsersMissingFields" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -126,48 +126,18 @@
     <t>{"Address1":"12234","Address2":"ABC Apt 12","City":"Farmington Hills","State":"MI","Country":"USA"}</t>
   </si>
   <si>
-    <t>Bauwa</t>
-  </si>
-  <si>
-    <t>abcr@xyz.com</t>
-  </si>
-  <si>
-    <t>PT9815</t>
-  </si>
-  <si>
-    <t>PT3732</t>
-  </si>
-  <si>
-    <t>PT1214</t>
-  </si>
-  <si>
-    <t>Shanta</t>
-  </si>
-  <si>
     <t>Prasad</t>
   </si>
   <si>
-    <t>Kersan</t>
-  </si>
-  <si>
     <t>Pillay</t>
   </si>
   <si>
-    <t>Celeste</t>
-  </si>
-  <si>
     <t>Viviers</t>
   </si>
   <si>
-    <t>Lester</t>
-  </si>
-  <si>
     <t>Williams</t>
   </si>
   <si>
-    <t>Ananta</t>
-  </si>
-  <si>
     <t>{"Address1":"32234","Address2":"XYZ Apt 12","City":"Cherry Hills","State":"AZ","Country":"USA"}</t>
   </si>
   <si>
@@ -202,6 +172,36 @@
   </si>
   <si>
     <t>abec@xyz.com</t>
+  </si>
+  <si>
+    <t>abcs@xyz.com</t>
+  </si>
+  <si>
+    <t>Sneha</t>
+  </si>
+  <si>
+    <t>Shane</t>
+  </si>
+  <si>
+    <t>Kirti</t>
+  </si>
+  <si>
+    <t>Shaun</t>
+  </si>
+  <si>
+    <t>Duncan</t>
+  </si>
+  <si>
+    <t>Priya</t>
+  </si>
+  <si>
+    <t>PT2630</t>
+  </si>
+  <si>
+    <t>PT5248</t>
+  </si>
+  <si>
+    <t>PT6346</t>
   </si>
 </sst>
 </file>
@@ -566,181 +566,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D28179-4852-4145-A51B-24A4D125D0CC}">
-  <dimension ref="A1:L4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2">
-        <v>1234567789</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3">
-        <v>1234567079</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>1234567789</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B0E6099-4721-446B-96B8-BA606B048C7A}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{2A71B001-FC2A-4C22-8ED9-B303CEC81AB0}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{CF97EE2B-3E10-4525-871E-4CC93041E906}"/>
-    <hyperlink ref="H3" r:id="rId4" xr:uid="{B7F072E7-0B76-4348-851B-1808A0AE1443}"/>
-    <hyperlink ref="E4" r:id="rId5" xr:uid="{1AD8AE8F-3951-47A6-A82F-DA8C8D69A8CA}"/>
-    <hyperlink ref="H4" r:id="rId6" xr:uid="{2648BEB7-0504-4A8F-9D4A-8920C651CA5E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018416D0-CD08-4368-A6CA-F452658D0032}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -795,10 +625,10 @@
     </row>
     <row r="2" spans="1:12" ht="103.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>31</v>
@@ -830,13 +660,13 @@
     </row>
     <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D3">
         <v>1234567789</v>
@@ -851,7 +681,7 @@
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
@@ -865,13 +695,13 @@
     </row>
     <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>1234567789</v>
@@ -886,13 +716,13 @@
         <v>14</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="I4" t="s">
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -900,13 +730,13 @@
     </row>
     <row r="5" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D5">
         <v>1234567789</v>
@@ -935,13 +765,13 @@
     </row>
     <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="D6">
         <v>1234567789</v>
@@ -986,11 +816,181 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D28179-4852-4145-A51B-24A4D125D0CC}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2">
+        <v>1234567789</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1234067089</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>1234567789</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{1B0E6099-4721-446B-96B8-BA606B048C7A}"/>
+    <hyperlink ref="H2" r:id="rId2" xr:uid="{2A71B001-FC2A-4C22-8ED9-B303CEC81AB0}"/>
+    <hyperlink ref="E3" r:id="rId3" xr:uid="{CF97EE2B-3E10-4525-871E-4CC93041E906}"/>
+    <hyperlink ref="H3" r:id="rId4" xr:uid="{B7F072E7-0B76-4348-851B-1808A0AE1443}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{1AD8AE8F-3951-47A6-A82F-DA8C8D69A8CA}"/>
+    <hyperlink ref="H4" r:id="rId6" xr:uid="{2648BEB7-0504-4A8F-9D4A-8920C651CA5E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1388D853-2EA6-4F5E-8015-64E1939A51CA}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1068,31 +1068,31 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B3" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>1234563789</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="G3" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="I3" t="s">
         <v>15</v>
       </c>
       <c r="J3" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -1113,8 +1113,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02DADCBE-48A3-4DC0-A2AB-73723BC94A41}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
final commit by Shilpi
</commit_message>
<xml_diff>
--- a/src/test/resources/exceldata/UsersAPI.xlsx
+++ b/src/test/resources/exceldata/UsersAPI.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\star\git\DieticianAPI-Hackathon\src\test\resources\exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6B8DBFD-AE0D-4B7B-A6A7-5A0C0FBDE8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDB8431-0288-4A80-BC09-DB8C67EEC865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E023EB60-0E3C-4029-8CA2-D4C7A83D16A1}"/>
   </bookViews>
   <sheets>
     <sheet name="PostUsers" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -174,27 +174,6 @@
     <t>abec@xyz.com</t>
   </si>
   <si>
-    <t>abcs@xyz.com</t>
-  </si>
-  <si>
-    <t>Sneha</t>
-  </si>
-  <si>
-    <t>Shane</t>
-  </si>
-  <si>
-    <t>Kirti</t>
-  </si>
-  <si>
-    <t>Shaun</t>
-  </si>
-  <si>
-    <t>Duncan</t>
-  </si>
-  <si>
-    <t>Priya</t>
-  </si>
-  <si>
     <t>PT2630</t>
   </si>
   <si>
@@ -202,12 +181,34 @@
   </si>
   <si>
     <t>PT6346</t>
+  </si>
+  <si>
+    <t>Kirtii</t>
+  </si>
+  <si>
+    <t>Shaneew</t>
+  </si>
+  <si>
+    <t>Shaunre</t>
+  </si>
+  <si>
+    <t>Duncantt</t>
+  </si>
+  <si>
+    <t>Priyate</t>
+  </si>
+  <si>
+    <t>Kiran</t>
+  </si>
+  <si>
+    <t>abct@xyz.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -569,20 +570,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018416D0-CD08-4368-A6CA-F452658D0032}">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="23" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.77734375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.77734375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -657,10 +658,11 @@
       <c r="K2" t="s">
         <v>28</v>
       </c>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>33</v>
@@ -692,10 +694,11 @@
       <c r="K3" t="s">
         <v>28</v>
       </c>
+      <c r="L3"/>
     </row>
     <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -727,10 +730,11 @@
       <c r="K4">
         <v>1</v>
       </c>
+      <c r="L4"/>
     </row>
     <row r="5" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -762,10 +766,11 @@
       <c r="K5" t="s">
         <v>28</v>
       </c>
+      <c r="L5"/>
     </row>
     <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
@@ -797,6 +802,7 @@
       <c r="K6" t="s">
         <v>28</v>
       </c>
+      <c r="L6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -820,14 +826,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57D28179-4852-4145-A51B-24A4D125D0CC}">
   <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -870,7 +876,7 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -899,9 +905,7 @@
       <c r="K2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
-        <v>55</v>
-      </c>
+      <c r="L2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -911,7 +915,7 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>1234067089</v>
+        <v>1234097089</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>12</v>
@@ -934,9 +938,7 @@
       <c r="K3" t="s">
         <v>29</v>
       </c>
-      <c r="L3" t="s">
-        <v>56</v>
-      </c>
+      <c r="L3"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -949,7 +951,7 @@
         <v>1234567789</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="F4" t="s">
         <v>13</v>
@@ -969,9 +971,7 @@
       <c r="K4" t="s">
         <v>30</v>
       </c>
-      <c r="L4" t="s">
-        <v>57</v>
-      </c>
+      <c r="L4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -996,7 +996,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1119,8 +1119,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="11.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>